<commit_message>
This is the 10th commit
</commit_message>
<xml_diff>
--- a/src/test/java/com/gurukula/testData/BranchDetails.xlsx
+++ b/src/test/java/com/gurukula/testData/BranchDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biswa.ranjan1\eclipse-workspace\Gurukulav0.1\src\test\java\com\gurukula\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BFE86D-B900-4933-9ACB-AEDF4164A16C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E44696-0075-4F19-A77E-85131967EE54}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1C7CE496-BBD7-49C1-9162-99EB5B1C4696}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <t>BranchCode</t>
   </si>
   <si>
-    <t>Utrech</t>
+    <t>Utrecht</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>